<commit_message>
Check-in the new changes
New  class added related to pageobject, testscript and databaseScript
</commit_message>
<xml_diff>
--- a/src/main/resource/configFile/testData.xlsx
+++ b/src/main/resource/configFile/testData.xlsx
@@ -3,22 +3,23 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Adobe_Workspace\uiFramework\src\main\resource\configFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CF12A3-8BF1-4F6B-8F3D-168CB9801617}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1769A06D-988B-4C6C-83E9-61746B606410}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C3114F97-09E3-4831-902E-4A7DCF698B5D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{C3114F97-09E3-4831-902E-4A7DCF698B5D}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="UpdateResult" sheetId="2" r:id="rId2"/>
+    <sheet name="loginData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>TestName</t>
   </si>
@@ -77,14 +78,37 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>StartLoginTest</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>runmode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>testname@gmail.com</t>
+  </si>
+  <si>
+    <t>testing@1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,16 +116,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,14 +147,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,7 +640,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E717D546-83AD-4E90-9E4D-85634B583307}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -623,4 +681,81 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85D9959D-B88E-45FF-8785-5CAF5F72FADB}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{05AFBBA2-83AB-452A-AB1A-7074535C8B1B}"/>
+    <hyperlink ref="B3:B4" r:id="rId2" display="testname@gmail.com" xr:uid="{CB31D865-29E9-47C0-889D-364BED1142B4}"/>
+    <hyperlink ref="C2" r:id="rId3" display="Adobe@1234" xr:uid="{32398A7B-8A33-49A4-BDB3-84DDAEB69008}"/>
+    <hyperlink ref="C3:C4" r:id="rId4" display="Adobe@1234" xr:uid="{4C454033-B8C7-459E-901B-B3617A2AE6F5}"/>
+    <hyperlink ref="C3" r:id="rId5" display="Adobe@1234" xr:uid="{145D158C-44CA-4C27-8070-D4DDE63708F7}"/>
+    <hyperlink ref="C4" r:id="rId6" display="Adobe@1234" xr:uid="{1C30D87E-6037-4729-B231-E324272DE0AE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>